<commit_message>
Script Completo, inserindo dados no banco
</commit_message>
<xml_diff>
--- a/transicao.xlsx
+++ b/transicao.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Eventos Transicao" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eventos Transicao" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -449,7 +449,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -794,7 +794,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -884,7 +884,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -914,7 +914,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2023-06-06 09:11:21</t>
+          <t>2023-06-06 12:40:00</t>
         </is>
       </c>
     </row>

</xml_diff>